<commit_message>
limpieza de codigo y comentarios añadidos.
</commit_message>
<xml_diff>
--- a/PreRegla3.xlsx
+++ b/PreRegla3.xlsx
@@ -14,9 +14,9 @@
   <definedNames>
     <definedName name="testSudoku" localSheetId="1">PostRegla3_fila!$A$1:$J$9</definedName>
     <definedName name="testSudoku" localSheetId="0">PreRegla3!$A$1:$J$9</definedName>
-    <definedName name="testSudoku_1" localSheetId="1">PostRegla3_fila!$A$14:$J$22</definedName>
-    <definedName name="testSudoku_2" localSheetId="1">PostRegla3_fila!$L$14:$U$22</definedName>
-    <definedName name="testSudoku_3" localSheetId="1">PostRegla3_fila!$L$24:$U$32</definedName>
+    <definedName name="testSudoku_3" localSheetId="1">PostRegla3_fila!$L$15:$U$23</definedName>
+    <definedName name="testSudoku_4" localSheetId="1">PostRegla3_fila!$L$28:$U$36</definedName>
+    <definedName name="testSudoku_5" localSheetId="1">PostRegla3_fila!$L$1:$U$9</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -56,7 +56,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="testSudoku2" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="3" name="testSudoku4" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\Alvaro\Desktop\testSudoku.txt" decimal="," thousands="." tab="0" delimiter="|">
       <textFields count="10">
         <textField/>
@@ -72,7 +72,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="testSudoku3" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="4" name="testSudoku5" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\Alvaro\Desktop\testSudoku.txt" decimal="," thousands="." tab="0" delimiter="|">
       <textFields count="10">
         <textField/>
@@ -88,8 +88,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="testSudoku4" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="C:\Users\Alvaro\Desktop\testSudoku.txt" decimal="," thousands="." tab="0" delimiter="|">
+  <connection id="5" name="testSudoku6" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Alvaro\Desktop\testSudoku.txt" decimal="," thousands="." delimiter="|">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="58">
   <si>
     <t>[5,8]</t>
   </si>
@@ -182,13 +182,106 @@
     <t>[3,5,7]</t>
   </si>
   <si>
-    <t>[7,9]</t>
-  </si>
-  <si>
-    <t>[2,7,9]</t>
-  </si>
-  <si>
-    <t>[1,7,9]</t>
+    <t>[1,6,8]</t>
+  </si>
+  <si>
+    <t>[1,3,5,8]</t>
+  </si>
+  <si>
+    <t>[4,6,7,8,9]</t>
+  </si>
+  <si>
+    <t>[4,5,6,7,8,9]</t>
+  </si>
+  <si>
+    <t>[2,3,5,7,8,9]</t>
+  </si>
+  <si>
+    <t>[2,3,5,7,9]</t>
+  </si>
+  <si>
+    <t>[3,4,5,8]</t>
+  </si>
+  <si>
+    <t>[3,4,5,6]</t>
+  </si>
+  <si>
+    <t>[4,5,6,8]</t>
+  </si>
+  <si>
+    <t>[1,4,5,8]</t>
+  </si>
+  <si>
+    <t>[1,2,9]</t>
+  </si>
+  <si>
+    <t>[1,4,9]</t>
+  </si>
+  <si>
+    <t>[1,4,6,9]</t>
+  </si>
+  <si>
+    <t>[2,7,8,9]</t>
+  </si>
+  <si>
+    <t>[1,2,3,5,8,9]</t>
+  </si>
+  <si>
+    <t>[2,3,5,6,8]</t>
+  </si>
+  <si>
+    <t>[1,2,3,5,9]</t>
+  </si>
+  <si>
+    <t>[1,4,5,7,9]</t>
+  </si>
+  <si>
+    <t>[4,5,6,7]</t>
+  </si>
+  <si>
+    <t>[1,4,5,6,9]</t>
+  </si>
+  <si>
+    <t>[1,5,8,9]</t>
+  </si>
+  <si>
+    <t>[1,5,9]</t>
+  </si>
+  <si>
+    <t>[3,7,8,9]</t>
+  </si>
+  <si>
+    <t>[2,3,5,7]</t>
+  </si>
+  <si>
+    <t>[3,5,7,8,9]</t>
+  </si>
+  <si>
+    <t>[2,5,8,9]</t>
+  </si>
+  <si>
+    <t>[3,6,7,8]</t>
+  </si>
+  <si>
+    <t>[5,6,7,8]</t>
+  </si>
+  <si>
+    <t>[1,2,3,5,7]</t>
+  </si>
+  <si>
+    <t>[1,2,3,4,5,7]</t>
+  </si>
+  <si>
+    <t>[3,4,5,7,8]</t>
+  </si>
+  <si>
+    <t>[3,4,5,7]</t>
+  </si>
+  <si>
+    <t>[2,4,5,8]</t>
+  </si>
+  <si>
+    <t>[4,5,9]</t>
   </si>
 </sst>
 </file>
@@ -258,19 +351,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="testSudoku_3" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="testSudoku_5" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="testSudoku_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="testSudoku_4" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="testSudoku_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="testSudoku" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="testSudoku" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="testSudoku_3" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -847,23 +940,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
     <col min="12" max="12" width="9.7109375" customWidth="1"/>
     <col min="13" max="13" width="8.140625" customWidth="1"/>
     <col min="14" max="14" width="11.28515625" customWidth="1"/>
@@ -876,8 +968,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
-        <v>6</v>
+      <c r="A1" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -894,8 +986,8 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2">
-        <v>1</v>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="H1" s="2">
         <v>9</v>
@@ -933,31 +1025,31 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2">
-        <v>3</v>
-      </c>
-      <c r="H2" s="2">
-        <v>6</v>
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>3</v>
@@ -989,16 +1081,16 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -1007,13 +1099,13 @@
         <v>6</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2">
         <v>2</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>9</v>
@@ -1054,22 +1146,22 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2">
         <v>7</v>
       </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>4</v>
+      <c r="F4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="H4" s="1">
         <v>8</v>
       </c>
-      <c r="I4" s="1">
-        <v>6</v>
+      <c r="I4" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="L4" s="1">
         <v>5</v>
@@ -1101,31 +1193,31 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2">
-        <v>6</v>
+        <v>38</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1">
-        <v>9</v>
+        <v>40</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>12</v>
@@ -1166,13 +1258,13 @@
         <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -1212,8 +1304,8 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>3</v>
+      <c r="A7" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
@@ -1224,20 +1316,20 @@
       <c r="D7" s="1">
         <v>6</v>
       </c>
-      <c r="E7" s="1">
-        <v>2</v>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L7" s="2">
         <v>3</v>
@@ -1269,31 +1361,31 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
+      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E8" s="1">
         <v>9</v>
       </c>
-      <c r="F8" s="1">
-        <v>4</v>
+      <c r="F8" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="2">
-        <v>3</v>
-      </c>
-      <c r="I8" s="2">
-        <v>2</v>
+        <v>54</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>21</v>
@@ -1345,11 +1437,11 @@
       <c r="G9" s="2">
         <v>6</v>
       </c>
-      <c r="H9" s="2">
-        <v>4</v>
+      <c r="H9" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="L9" s="2">
         <v>2</v>
@@ -1376,771 +1468,6 @@
         <v>4</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1">
-        <v>4</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2">
-        <v>9</v>
-      </c>
-      <c r="I14" s="2">
-        <v>7</v>
-      </c>
-      <c r="L14" s="1">
-        <v>6</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>2</v>
-      </c>
-      <c r="O14" s="1">
-        <v>4</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R14" s="1">
-        <v>1</v>
-      </c>
-      <c r="S14" s="1">
-        <v>9</v>
-      </c>
-      <c r="T14" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="2">
-        <v>3</v>
-      </c>
-      <c r="H15" s="2">
-        <v>6</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R15" s="1">
-        <v>3</v>
-      </c>
-      <c r="S15" s="1">
-        <v>6</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>6</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>2</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M16" s="1">
-        <v>3</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>6</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S16" s="1">
-        <v>2</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="2">
-        <v>7</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1">
-        <v>4</v>
-      </c>
-      <c r="H17" s="1">
-        <v>8</v>
-      </c>
-      <c r="I17" s="1">
-        <v>6</v>
-      </c>
-      <c r="L17" s="1">
-        <v>5</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N17" s="1">
-        <v>3</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P17" s="1">
-        <v>7</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>1</v>
-      </c>
-      <c r="R17" s="1">
-        <v>4</v>
-      </c>
-      <c r="S17" s="1">
-        <v>8</v>
-      </c>
-      <c r="T17" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="2">
-        <v>6</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="1">
-        <v>9</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P18" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R18" s="1">
-        <v>9</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="2">
-        <v>4</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="1">
-        <v>2</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="1">
-        <v>3</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="1">
-        <v>6</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P19" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R19" s="1">
-        <v>2</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T19" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2">
-        <v>4</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="1">
-        <v>6</v>
-      </c>
-      <c r="E20" s="1">
-        <v>2</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L20" s="1">
-        <v>3</v>
-      </c>
-      <c r="M20" s="1">
-        <v>4</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O20" s="1">
-        <v>6</v>
-      </c>
-      <c r="P20" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S20" s="1">
-        <v>1</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2">
-        <v>6</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1">
-        <v>9</v>
-      </c>
-      <c r="F21" s="1">
-        <v>4</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="2">
-        <v>3</v>
-      </c>
-      <c r="I21" s="2">
-        <v>2</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N21" s="1">
-        <v>6</v>
-      </c>
-      <c r="O21" s="1">
-        <v>1</v>
-      </c>
-      <c r="P21" s="1">
-        <v>9</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>4</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S21" s="1">
-        <v>3</v>
-      </c>
-      <c r="T21" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>2</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="1">
-        <v>8</v>
-      </c>
-      <c r="G22" s="2">
-        <v>6</v>
-      </c>
-      <c r="H22" s="2">
-        <v>4</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="1">
-        <v>2</v>
-      </c>
-      <c r="M22" s="1">
-        <v>1</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>8</v>
-      </c>
-      <c r="R22" s="1">
-        <v>6</v>
-      </c>
-      <c r="S22" s="1">
-        <v>4</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L24">
-        <v>6</v>
-      </c>
-      <c r="M24" t="s">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>2</v>
-      </c>
-      <c r="O24">
-        <v>4</v>
-      </c>
-      <c r="P24" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>2</v>
-      </c>
-      <c r="R24">
-        <v>1</v>
-      </c>
-      <c r="S24">
-        <v>9</v>
-      </c>
-      <c r="T24">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L25" t="s">
-        <v>3</v>
-      </c>
-      <c r="M25" t="s">
-        <v>4</v>
-      </c>
-      <c r="N25" t="s">
-        <v>5</v>
-      </c>
-      <c r="O25" t="s">
-        <v>6</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>7</v>
-      </c>
-      <c r="R25">
-        <v>3</v>
-      </c>
-      <c r="S25">
-        <v>6</v>
-      </c>
-      <c r="T25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L26" t="s">
-        <v>9</v>
-      </c>
-      <c r="M26">
-        <v>3</v>
-      </c>
-      <c r="N26" t="s">
-        <v>10</v>
-      </c>
-      <c r="O26" t="s">
-        <v>4</v>
-      </c>
-      <c r="P26" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>6</v>
-      </c>
-      <c r="R26" t="s">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>2</v>
-      </c>
-      <c r="T26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L27">
-        <v>5</v>
-      </c>
-      <c r="M27" t="s">
-        <v>11</v>
-      </c>
-      <c r="N27">
-        <v>3</v>
-      </c>
-      <c r="O27" t="s">
-        <v>11</v>
-      </c>
-      <c r="P27">
-        <v>7</v>
-      </c>
-      <c r="Q27">
-        <v>1</v>
-      </c>
-      <c r="R27">
-        <v>4</v>
-      </c>
-      <c r="S27">
-        <v>8</v>
-      </c>
-      <c r="T27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L28" t="s">
-        <v>12</v>
-      </c>
-      <c r="M28" t="s">
-        <v>13</v>
-      </c>
-      <c r="N28" t="s">
-        <v>12</v>
-      </c>
-      <c r="O28" t="s">
-        <v>14</v>
-      </c>
-      <c r="P28">
-        <v>6</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>15</v>
-      </c>
-      <c r="R28">
-        <v>9</v>
-      </c>
-      <c r="S28" t="s">
-        <v>16</v>
-      </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L29" t="s">
-        <v>17</v>
-      </c>
-      <c r="M29">
-        <v>6</v>
-      </c>
-      <c r="N29" t="s">
-        <v>17</v>
-      </c>
-      <c r="O29" t="s">
-        <v>18</v>
-      </c>
-      <c r="P29">
-        <v>4</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>19</v>
-      </c>
-      <c r="R29">
-        <v>2</v>
-      </c>
-      <c r="S29" t="s">
-        <v>16</v>
-      </c>
-      <c r="T29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L30">
-        <v>3</v>
-      </c>
-      <c r="M30">
-        <v>4</v>
-      </c>
-      <c r="N30" t="s">
-        <v>4</v>
-      </c>
-      <c r="O30">
-        <v>6</v>
-      </c>
-      <c r="P30">
-        <v>2</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>16</v>
-      </c>
-      <c r="R30" t="s">
-        <v>20</v>
-      </c>
-      <c r="S30">
-        <v>1</v>
-      </c>
-      <c r="T30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L31" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" t="s">
-        <v>20</v>
-      </c>
-      <c r="N31">
-        <v>6</v>
-      </c>
-      <c r="O31">
-        <v>1</v>
-      </c>
-      <c r="P31">
-        <v>9</v>
-      </c>
-      <c r="Q31">
-        <v>4</v>
-      </c>
-      <c r="R31" t="s">
-        <v>20</v>
-      </c>
-      <c r="S31">
-        <v>3</v>
-      </c>
-      <c r="T31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L32">
-        <v>2</v>
-      </c>
-      <c r="M32">
-        <v>1</v>
-      </c>
-      <c r="N32" t="s">
-        <v>22</v>
-      </c>
-      <c r="O32" t="s">
-        <v>23</v>
-      </c>
-      <c r="P32" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q32">
-        <v>8</v>
-      </c>
-      <c r="R32">
-        <v>6</v>
-      </c>
-      <c r="S32">
-        <v>4</v>
-      </c>
-      <c r="T32" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>